<commit_message>
add paymnet in admina nd shipping cal
</commit_message>
<xml_diff>
--- a/public_html/export/country-master.xlsx
+++ b/public_html/export/country-master.xlsx
@@ -75,15 +75,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>